<commit_message>
Migration Update + DB Updtae + Logs
</commit_message>
<xml_diff>
--- a/Logs/7th Week Logs.xlsx
+++ b/Logs/7th Week Logs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF229BC7-1B07-4E38-97CA-CFF950AB203F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1186E63B-D2CE-4812-8FB5-6B374A5A29C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2088" yWindow="948" windowWidth="11520" windowHeight="11412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -841,7 +841,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,14 +1027,30 @@
       <c r="K10" s="41"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="38"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="20"/>
+      <c r="B11" s="38">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>43539</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.4375</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F11" s="4">
+        <v>15</v>
+      </c>
+      <c r="G11" s="12">
+        <v>180</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="41"/>
     </row>
@@ -1144,7 +1160,7 @@
       </c>
       <c r="G20" s="18">
         <f>SUM(G8:G19)</f>
-        <v>695</v>
+        <v>875</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>

</xml_diff>